<commit_message>
Adds project version 1
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project_gnew\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project_gnew\project_new\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F7B74D-00B7-4D4C-8477-67A52E6D49D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E768085D-46B3-4034-B388-C036DA78EF92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="840" windowWidth="14550" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="780" windowWidth="14535" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2122" uniqueCount="1184">
   <si>
     <t>rec.pres.</t>
   </si>
@@ -3743,12 +3744,15 @@
   <si>
     <t>trainstations</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -3779,6 +3783,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -4000,7 +4010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4108,6 +4118,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5300,8 +5319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV321"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C226" sqref="C226"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5517,7 +5536,9 @@
         <v>20</v>
       </c>
       <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="N3" s="8" t="s">
+        <v>1183</v>
+      </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
@@ -5599,7 +5620,9 @@
         <v>26</v>
       </c>
       <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="N4" s="8" t="s">
+        <v>1183</v>
+      </c>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
@@ -7419,7 +7442,7 @@
         <v>116</v>
       </c>
       <c r="I26" s="15"/>
-      <c r="J26" s="15" t="s">
+      <c r="J26" s="47" t="s">
         <v>1150</v>
       </c>
       <c r="K26" s="15" t="s">
@@ -7669,7 +7692,7 @@
         <v>127</v>
       </c>
       <c r="I29" s="15"/>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="47" t="s">
         <v>1152</v>
       </c>
       <c r="K29" s="15" t="s">
@@ -7835,7 +7858,7 @@
         <v>135</v>
       </c>
       <c r="I31" s="15"/>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="47" t="s">
         <v>1153</v>
       </c>
       <c r="K31" s="15" t="s">
@@ -8083,7 +8106,7 @@
       <c r="I34" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="J34" s="29" t="s">
+      <c r="J34" s="48" t="s">
         <v>1154</v>
       </c>
       <c r="K34" s="29" t="s">
@@ -9443,7 +9466,7 @@
       <c r="I50" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="J50" s="11" t="s">
+      <c r="J50" s="49" t="s">
         <v>1156</v>
       </c>
       <c r="K50" s="11" t="s">
@@ -9529,7 +9552,7 @@
       <c r="I51" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="J51" s="15" t="s">
+      <c r="J51" s="47" t="s">
         <v>1136</v>
       </c>
       <c r="K51" s="15" t="s">

</xml_diff>